<commit_message>
Added 1p and 1q cnas.
</commit_message>
<xml_diff>
--- a/tables/CNV_TFPN_cnvkit.xlsx
+++ b/tables/CNV_TFPN_cnvkit.xlsx
@@ -1037,11 +1037,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW2" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX2" s="20" t="n">
-        <v>0</v>
+      <c r="AW2" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX2" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY2" s="20" t="n">
         <v>0</v>
@@ -1243,11 +1247,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW3" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX3" s="20" t="n">
-        <v>0</v>
+      <c r="AW3" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX3" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY3" s="20" t="n">
         <v>0</v>
@@ -1450,11 +1458,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW4" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX4" s="20" t="n">
-        <v>0</v>
+      <c r="AW4" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX4" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY4" s="20" t="n">
         <v>0</v>
@@ -1657,11 +1669,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW5" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX5" s="20" t="n">
-        <v>0</v>
+      <c r="AW5" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX5" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY5" s="20" t="n">
         <v>0</v>
@@ -1864,11 +1880,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW6" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX6" s="20" t="n">
-        <v>0</v>
+      <c r="AW6" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX6" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY6" s="20" t="n">
         <v>0</v>
@@ -2069,11 +2089,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW7" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX7" s="20" t="n">
-        <v>0</v>
+      <c r="AW7" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX7" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY7" s="20" t="n">
         <v>0</v>
@@ -2272,11 +2296,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW8" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX8" s="20" t="n">
-        <v>0</v>
+      <c r="AW8" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX8" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY8" s="20" t="n">
         <v>0</v>
@@ -2479,11 +2507,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW9" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX9" s="20" t="n">
-        <v>0</v>
+      <c r="AW9" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX9" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY9" s="20" t="n">
         <v>0</v>
@@ -2686,11 +2718,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW10" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX10" s="20" t="n">
-        <v>0</v>
+      <c r="AW10" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX10" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY10" s="20" t="n">
         <v>0</v>
@@ -2898,11 +2934,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW11" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX11" s="20" t="n">
-        <v>0</v>
+      <c r="AW11" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX11" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY11" s="20" t="n">
         <v>0</v>
@@ -3105,11 +3145,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW12" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX12" s="20" t="n">
-        <v>0</v>
+      <c r="AW12" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX12" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY12" s="20" t="n">
         <v>0</v>
@@ -3317,11 +3361,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW13" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX13" s="20" t="n">
-        <v>0</v>
+      <c r="AW13" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX13" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY13" s="20" t="n">
         <v>0</v>
@@ -3525,11 +3573,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW14" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX14" s="20" t="n">
-        <v>0</v>
+      <c r="AW14" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX14" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY14" s="20" t="n">
         <v>0</v>
@@ -3728,11 +3780,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW15" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX15" s="20" t="n">
-        <v>0</v>
+      <c r="AW15" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX15" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY15" s="20" t="n">
         <v>0</v>
@@ -3935,11 +3991,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW16" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX16" s="20" t="n">
-        <v>0</v>
+      <c r="AW16" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX16" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY16" s="20" t="n">
         <v>0</v>
@@ -4138,11 +4198,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW17" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX17" s="20" t="n">
-        <v>0</v>
+      <c r="AW17" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX17" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY17" s="20" t="n">
         <v>0</v>
@@ -4345,11 +4409,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW18" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX18" s="20" t="n">
-        <v>0</v>
+      <c r="AW18" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX18" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY18" s="20" t="n">
         <v>0</v>
@@ -4552,11 +4620,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW19" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX19" s="20" t="n">
-        <v>0</v>
+      <c r="AW19" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX19" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY19" s="20" t="n">
         <v>0</v>
@@ -4759,11 +4831,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW20" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX20" s="20" t="n">
-        <v>0</v>
+      <c r="AW20" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX20" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY20" s="20" t="n">
         <v>0</v>
@@ -4962,11 +5038,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW21" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX21" s="20" t="n">
-        <v>0</v>
+      <c r="AW21" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX21" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY21" s="20" t="n">
         <v>0</v>
@@ -5174,11 +5254,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW22" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX22" s="20" t="n">
-        <v>0</v>
+      <c r="AW22" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX22" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY22" s="20" t="n">
         <v>0</v>
@@ -5381,11 +5465,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW23" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX23" s="20" t="n">
-        <v>0</v>
+      <c r="AW23" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX23" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY23" s="20" t="n">
         <v>0</v>
@@ -5588,11 +5676,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW24" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX24" s="20" t="n">
-        <v>0</v>
+      <c r="AW24" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX24" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY24" s="20" t="n">
         <v>0</v>
@@ -5791,11 +5883,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW25" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX25" s="20" t="n">
-        <v>0</v>
+      <c r="AW25" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX25" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY25" s="20" t="n">
         <v>0</v>
@@ -5992,11 +6088,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW26" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX26" s="20" t="n">
-        <v>0</v>
+      <c r="AW26" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX26" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY26" s="20" t="n">
         <v>0</v>
@@ -6195,11 +6295,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW27" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX27" s="20" t="n">
-        <v>0</v>
+      <c r="AW27" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX27" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY27" s="20" t="n">
         <v>0</v>
@@ -6398,11 +6502,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW28" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX28" s="20" t="n">
-        <v>0</v>
+      <c r="AW28" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX28" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY28" s="20" t="n">
         <v>0</v>
@@ -6601,11 +6709,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW29" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX29" s="20" t="n">
-        <v>0</v>
+      <c r="AW29" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX29" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY29" s="20" t="n">
         <v>0</v>
@@ -6802,11 +6914,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW30" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX30" s="20" t="n">
-        <v>0</v>
+      <c r="AW30" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX30" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY30" s="20" t="n">
         <v>0</v>
@@ -7014,11 +7130,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW31" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX31" s="20" t="n">
-        <v>0</v>
+      <c r="AW31" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX31" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY31" s="20" t="n">
         <v>0</v>
@@ -7221,11 +7341,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW32" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX32" s="20" t="n">
-        <v>0</v>
+      <c r="AW32" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX32" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY32" s="20" t="n">
         <v>0</v>
@@ -7424,11 +7548,15 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="AW33" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX33" s="20" t="n">
-        <v>0</v>
+      <c r="AW33" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX33" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY33" s="20" t="n">
         <v>0</v>
@@ -7636,11 +7764,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW34" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX34" s="20" t="n">
-        <v>0</v>
+      <c r="AW34" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX34" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY34" s="20" t="n">
         <v>0</v>
@@ -7843,11 +7975,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW35" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX35" s="20" t="n">
-        <v>0</v>
+      <c r="AW35" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX35" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY35" s="20" t="n">
         <v>0</v>
@@ -8046,11 +8182,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW36" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX36" s="20" t="n">
-        <v>0</v>
+      <c r="AW36" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX36" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY36" s="20" t="n">
         <v>0</v>
@@ -8254,11 +8394,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW37" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX37" s="20" t="n">
-        <v>0</v>
+      <c r="AW37" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX37" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY37" s="20" t="n">
         <v>0</v>
@@ -8457,11 +8601,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW38" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX38" s="20" t="n">
-        <v>0</v>
+      <c r="AW38" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX38" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY38" s="20" t="n">
         <v>0</v>
@@ -8660,11 +8808,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW39" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX39" s="20" t="n">
-        <v>0</v>
+      <c r="AW39" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX39" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY39" s="20" t="n">
         <v>0</v>
@@ -8863,11 +9015,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW40" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX40" s="20" t="n">
-        <v>0</v>
+      <c r="AW40" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX40" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY40" s="20" t="n">
         <v>0</v>
@@ -9070,11 +9226,15 @@
           <t>FN</t>
         </is>
       </c>
-      <c r="AW41" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX41" s="20" t="n">
-        <v>0</v>
+      <c r="AW41" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX41" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY41" s="20" t="n">
         <v>0</v>
@@ -9278,11 +9438,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW42" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX42" s="20" t="n">
-        <v>0</v>
+      <c r="AW42" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX42" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY42" s="20" t="n">
         <v>0</v>
@@ -9485,11 +9649,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW43" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX43" s="20" t="n">
-        <v>0</v>
+      <c r="AW43" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX43" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY43" s="20" t="n">
         <v>0</v>
@@ -9692,11 +9860,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW44" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX44" s="20" t="n">
-        <v>0</v>
+      <c r="AW44" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX44" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY44" s="20" t="n">
         <v>0</v>
@@ -9899,11 +10071,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW45" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX45" s="20" t="n">
-        <v>0</v>
+      <c r="AW45" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX45" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY45" s="20" t="n">
         <v>0</v>
@@ -10106,11 +10282,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW46" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX46" s="20" t="n">
-        <v>0</v>
+      <c r="AW46" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX46" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY46" s="20" t="n">
         <v>0</v>
@@ -10309,11 +10489,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW47" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX47" s="20" t="n">
-        <v>0</v>
+      <c r="AW47" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX47" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY47" s="20" t="n">
         <v>0</v>
@@ -10516,11 +10700,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW48" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX48" s="20" t="n">
-        <v>0</v>
+      <c r="AW48" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX48" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY48" s="20" t="n">
         <v>0</v>
@@ -10729,11 +10917,15 @@
           <t>FP</t>
         </is>
       </c>
-      <c r="AW49" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX49" s="20" t="n">
-        <v>0</v>
+      <c r="AW49" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX49" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY49" s="20" t="n">
         <v>0</v>
@@ -10941,11 +11133,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW50" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX50" s="20" t="n">
-        <v>0</v>
+      <c r="AW50" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX50" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY50" s="20" t="n">
         <v>0</v>
@@ -11153,11 +11349,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW51" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX51" s="20" t="n">
-        <v>0</v>
+      <c r="AW51" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX51" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY51" s="20" t="n">
         <v>0</v>
@@ -11365,11 +11565,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW52" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX52" s="20" t="n">
-        <v>0</v>
+      <c r="AW52" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX52" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY52" s="20" t="n">
         <v>0</v>
@@ -11577,11 +11781,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW53" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX53" s="20" t="n">
-        <v>0</v>
+      <c r="AW53" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX53" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY53" s="20" t="n">
         <v>0</v>
@@ -11789,11 +11997,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW54" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX54" s="20" t="n">
-        <v>0</v>
+      <c r="AW54" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX54" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY54" s="20" t="n">
         <v>0</v>
@@ -12001,11 +12213,15 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="AW55" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX55" s="20" t="n">
-        <v>0</v>
+      <c r="AW55" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX55" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY55" s="20" t="n">
         <v>0</v>
@@ -12213,11 +12429,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW56" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX56" s="20" t="n">
-        <v>0</v>
+      <c r="AW56" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX56" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY56" s="20" t="n">
         <v>0</v>
@@ -12425,11 +12645,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW57" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX57" s="20" t="n">
-        <v>0</v>
+      <c r="AW57" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX57" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY57" s="20" t="n">
         <v>0</v>
@@ -12632,11 +12856,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW58" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX58" s="20" t="n">
-        <v>0</v>
+      <c r="AW58" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX58" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY58" s="20" t="n">
         <v>0</v>
@@ -12844,11 +13072,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW59" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX59" s="20" t="n">
-        <v>0</v>
+      <c r="AW59" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX59" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY59" s="20" t="n">
         <v>0</v>
@@ -13056,11 +13288,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW60" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX60" s="20" t="n">
-        <v>0</v>
+      <c r="AW60" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX60" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY60" s="20" t="n">
         <v>0</v>
@@ -13268,11 +13504,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW61" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX61" s="20" t="n">
-        <v>0</v>
+      <c r="AW61" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX61" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY61" s="20" t="n">
         <v>0</v>
@@ -13480,11 +13720,15 @@
           <t>FN</t>
         </is>
       </c>
-      <c r="AW62" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX62" s="20" t="n">
-        <v>0</v>
+      <c r="AW62" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX62" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY62" s="20" t="n">
         <v>0</v>
@@ -13697,11 +13941,15 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="AW63" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX63" s="20" t="n">
-        <v>0</v>
+      <c r="AW63" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX63" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY63" s="20" t="n">
         <v>0</v>
@@ -13909,11 +14157,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW64" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX64" s="20" t="n">
-        <v>0</v>
+      <c r="AW64" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX64" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
       </c>
       <c r="AY64" s="20" t="n">
         <v>0</v>
@@ -14121,11 +14373,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW65" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX65" s="20" t="n">
-        <v>0</v>
+      <c r="AW65" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX65" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY65" s="20" t="n">
         <v>0</v>
@@ -14333,11 +14589,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW66" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX66" s="20" t="n">
-        <v>0</v>
+      <c r="AW66" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX66" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY66" s="20" t="n">
         <v>0</v>
@@ -14545,11 +14805,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW67" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX67" s="20" t="n">
-        <v>0</v>
+      <c r="AW67" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX67" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY67" s="20" t="n">
         <v>0</v>
@@ -14757,11 +15021,15 @@
           <t>FN</t>
         </is>
       </c>
-      <c r="AW68" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX68" s="20" t="n">
-        <v>0</v>
+      <c r="AW68" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX68" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY68" s="20" t="n">
         <v>0</v>
@@ -14969,11 +15237,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW69" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX69" s="20" t="n">
-        <v>0</v>
+      <c r="AW69" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX69" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY69" s="20" t="n">
         <v>0</v>
@@ -15181,11 +15453,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW70" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX70" s="20" t="n">
-        <v>0</v>
+      <c r="AW70" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX70" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY70" s="20" t="n">
         <v>0</v>
@@ -15389,11 +15665,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW71" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX71" s="20" t="n">
-        <v>0</v>
+      <c r="AW71" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX71" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY71" s="20" t="n">
         <v>0</v>
@@ -15601,11 +15881,15 @@
           <t>FN</t>
         </is>
       </c>
-      <c r="AW72" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX72" s="20" t="n">
-        <v>0</v>
+      <c r="AW72" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX72" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY72" s="20" t="n">
         <v>0</v>
@@ -15813,11 +16097,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW73" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX73" s="20" t="n">
-        <v>0</v>
+      <c r="AW73" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX73" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY73" s="20" t="n">
         <v>0</v>
@@ -16025,11 +16313,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW74" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX74" s="20" t="n">
-        <v>0</v>
+      <c r="AW74" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX74" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY74" s="20" t="n">
         <v>0</v>
@@ -16237,11 +16529,15 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="AW75" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX75" s="20" t="n">
-        <v>0</v>
+      <c r="AW75" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX75" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY75" s="20" t="n">
         <v>0</v>
@@ -16449,11 +16745,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW76" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX76" s="20" t="n">
-        <v>1</v>
+      <c r="AW76" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX76" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
       </c>
       <c r="AY76" s="20" t="n">
         <v>0</v>
@@ -16661,11 +16961,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW77" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX77" s="20" t="n">
-        <v>1</v>
+      <c r="AW77" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX77" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
       </c>
       <c r="AY77" s="20" t="n">
         <v>0</v>
@@ -16873,11 +17177,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW78" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX78" s="20" t="n">
-        <v>1</v>
+      <c r="AW78" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX78" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
       </c>
       <c r="AY78" s="20" t="n">
         <v>0</v>
@@ -17085,11 +17393,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW79" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX79" s="20" t="n">
-        <v>0</v>
+      <c r="AW79" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX79" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY79" s="20" t="n">
         <v>0</v>
@@ -17297,11 +17609,15 @@
           <t>FN</t>
         </is>
       </c>
-      <c r="AW80" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX80" s="20" t="n">
-        <v>0</v>
+      <c r="AW80" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX80" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY80" s="20" t="n">
         <v>0</v>
@@ -17514,11 +17830,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW81" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX81" s="20" t="n">
-        <v>0</v>
+      <c r="AW81" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX81" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY81" s="20" t="n">
         <v>0</v>
@@ -17726,11 +18046,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW82" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX82" s="20" t="n">
-        <v>0</v>
+      <c r="AW82" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX82" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY82" s="20" t="n">
         <v>0</v>
@@ -17938,11 +18262,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW83" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX83" s="20" t="n">
-        <v>0</v>
+      <c r="AW83" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX83" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY83" s="20" t="n">
         <v>0</v>
@@ -18150,11 +18478,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW84" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX84" s="20" t="n">
-        <v>0</v>
+      <c r="AW84" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX84" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY84" s="20" t="n">
         <v>0</v>
@@ -18362,11 +18694,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW85" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX85" s="20" t="n">
-        <v>0</v>
+      <c r="AW85" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX85" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY85" s="20" t="n">
         <v>0</v>
@@ -18570,11 +18906,15 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="AW86" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX86" s="20" t="n">
-        <v>0</v>
+      <c r="AW86" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX86" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY86" s="20" t="n">
         <v>0</v>
@@ -18782,11 +19122,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW87" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX87" s="20" t="n">
-        <v>0</v>
+      <c r="AW87" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX87" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY87" s="20" t="n">
         <v>0</v>
@@ -18989,11 +19333,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW88" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX88" s="20" t="n">
-        <v>0</v>
+      <c r="AW88" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX88" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY88" s="20" t="n">
         <v>0</v>
@@ -19201,11 +19549,15 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="AW89" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX89" s="20" t="n">
-        <v>0</v>
+      <c r="AW89" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX89" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY89" s="20" t="n">
         <v>0</v>
@@ -19413,11 +19765,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW90" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX90" s="20" t="n">
-        <v>0</v>
+      <c r="AW90" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX90" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY90" s="20" t="n">
         <v>0</v>
@@ -19625,11 +19981,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW91" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX91" s="20" t="n">
-        <v>0</v>
+      <c r="AW91" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX91" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY91" s="20" t="n">
         <v>0</v>
@@ -19832,11 +20192,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW92" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX92" s="20" t="n">
-        <v>0</v>
+      <c r="AW92" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX92" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY92" s="20" t="n">
         <v>0</v>
@@ -20044,11 +20408,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW93" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX93" s="20" t="n">
-        <v>0</v>
+      <c r="AW93" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX93" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY93" s="20" t="n">
         <v>0</v>
@@ -20256,11 +20624,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW94" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX94" s="20" t="n">
-        <v>0</v>
+      <c r="AW94" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX94" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY94" s="20" t="n">
         <v>0</v>
@@ -20468,11 +20840,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW95" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX95" s="20" t="n">
-        <v>0</v>
+      <c r="AW95" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX95" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY95" s="20" t="n">
         <v>0</v>
@@ -20680,11 +21056,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW96" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX96" s="20" t="n">
-        <v>0</v>
+      <c r="AW96" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX96" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY96" s="20" t="n">
         <v>0</v>
@@ -20887,11 +21267,15 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="AW97" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX97" s="20" t="n">
-        <v>0</v>
+      <c r="AW97" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX97" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY97" s="20" t="n">
         <v>0</v>
@@ -21099,11 +21483,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW98" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX98" s="20" t="n">
-        <v>0</v>
+      <c r="AW98" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX98" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY98" s="20" t="n">
         <v>0</v>
@@ -21311,11 +21699,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW99" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX99" s="20" t="n">
-        <v>0</v>
+      <c r="AW99" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX99" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY99" s="20" t="n">
         <v>0</v>
@@ -21523,11 +21915,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW100" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX100" s="20" t="n">
-        <v>0</v>
+      <c r="AW100" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX100" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY100" s="20" t="n">
         <v>0</v>
@@ -21735,11 +22131,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW101" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX101" s="20" t="n">
-        <v>0</v>
+      <c r="AW101" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX101" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY101" s="20" t="n">
         <v>0</v>
@@ -21947,11 +22347,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW102" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX102" s="20" t="n">
-        <v>0</v>
+      <c r="AW102" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX102" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY102" s="20" t="n">
         <v>0</v>
@@ -22159,11 +22563,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW103" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX103" s="20" t="n">
-        <v>0</v>
+      <c r="AW103" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX103" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY103" s="20" t="n">
         <v>0</v>
@@ -22371,11 +22779,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW104" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX104" s="20" t="n">
-        <v>0</v>
+      <c r="AW104" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX104" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY104" s="20" t="n">
         <v>0</v>
@@ -22583,11 +22995,15 @@
           <t>FN</t>
         </is>
       </c>
-      <c r="AW105" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX105" s="20" t="n">
-        <v>0</v>
+      <c r="AW105" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX105" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY105" s="20" t="n">
         <v>0</v>
@@ -22800,11 +23216,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW106" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX106" s="20" t="n">
-        <v>0</v>
+      <c r="AW106" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX106" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY106" s="20" t="n">
         <v>0</v>
@@ -23012,11 +23432,15 @@
           <t>FN</t>
         </is>
       </c>
-      <c r="AW107" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX107" s="20" t="n">
-        <v>0</v>
+      <c r="AW107" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX107" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY107" s="20" t="n">
         <v>0</v>
@@ -23229,11 +23653,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW108" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX108" s="20" t="n">
-        <v>0</v>
+      <c r="AW108" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX108" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY108" s="20" t="n">
         <v>0</v>
@@ -23446,11 +23874,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW109" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX109" s="20" t="n">
-        <v>0</v>
+      <c r="AW109" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX109" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY109" s="20" t="n">
         <v>0</v>
@@ -23658,11 +24090,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW110" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX110" s="20" t="n">
-        <v>0</v>
+      <c r="AW110" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX110" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY110" s="20" t="n">
         <v>0</v>
@@ -23870,11 +24306,15 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="AW111" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX111" s="20" t="n">
-        <v>0</v>
+      <c r="AW111" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX111" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY111" s="20" t="n">
         <v>0</v>
@@ -24082,11 +24522,15 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="AW112" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX112" s="20" t="n">
-        <v>0</v>
+      <c r="AW112" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX112" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY112" s="20" t="n">
         <v>0</v>
@@ -24294,11 +24738,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW113" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX113" s="20" t="n">
-        <v>0</v>
+      <c r="AW113" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX113" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY113" s="20" t="n">
         <v>0</v>
@@ -24506,11 +24954,15 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="AW114" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX114" s="20" t="n">
-        <v>0</v>
+      <c r="AW114" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX114" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY114" s="20" t="n">
         <v>0</v>
@@ -24718,11 +25170,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW115" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX115" s="20" t="n">
-        <v>0</v>
+      <c r="AW115" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX115" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY115" s="20" t="n">
         <v>0</v>
@@ -24925,11 +25381,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW116" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX116" s="20" t="n">
-        <v>0</v>
+      <c r="AW116" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX116" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY116" s="20" t="n">
         <v>0</v>
@@ -25137,11 +25597,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW117" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX117" s="20" t="n">
-        <v>0</v>
+      <c r="AW117" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX117" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY117" s="20" t="n">
         <v>0</v>
@@ -25349,11 +25813,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW118" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX118" s="20" t="n">
-        <v>0</v>
+      <c r="AW118" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX118" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY118" s="20" t="n">
         <v>0</v>
@@ -25561,11 +26029,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW119" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX119" s="20" t="n">
-        <v>0</v>
+      <c r="AW119" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX119" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY119" s="20" t="n">
         <v>0</v>
@@ -25767,11 +26239,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW120" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX120" s="20" t="n">
-        <v>0</v>
+      <c r="AW120" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX120" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
       </c>
       <c r="AY120" s="20" t="n">
         <v>0</v>
@@ -25974,11 +26450,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW121" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX121" s="20" t="n">
-        <v>0</v>
+      <c r="AW121" s="20" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="AX121" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY121" s="20" t="n">
         <v>0</v>
@@ -26181,11 +26661,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW122" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX122" s="20" t="n">
-        <v>0</v>
+      <c r="AW122" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX122" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY122" s="20" t="n">
         <v>0</v>
@@ -26398,11 +26882,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW123" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX123" s="20" t="n">
-        <v>0</v>
+      <c r="AW123" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX123" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
       </c>
       <c r="AY123" s="20" t="n">
         <v>0</v>
@@ -26605,11 +27093,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW124" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX124" s="20" t="n">
-        <v>0</v>
+      <c r="AW124" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX124" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY124" s="20" t="n">
         <v>0</v>
@@ -26822,11 +27314,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW125" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX125" s="20" t="n">
-        <v>0</v>
+      <c r="AW125" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX125" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY125" s="20" t="n">
         <v>0</v>
@@ -27029,11 +27525,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW126" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX126" s="20" t="n">
-        <v>0</v>
+      <c r="AW126" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX126" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY126" s="20" t="n">
         <v>0</v>
@@ -27236,11 +27736,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW127" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX127" s="20" t="n">
-        <v>0</v>
+      <c r="AW127" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX127" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY127" s="20" t="n">
         <v>0</v>
@@ -27453,11 +27957,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW128" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX128" s="20" t="n">
-        <v>0</v>
+      <c r="AW128" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX128" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY128" s="20" t="n">
         <v>0</v>
@@ -27660,11 +28168,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW129" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX129" s="20" t="n">
-        <v>0</v>
+      <c r="AW129" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX129" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY129" s="20" t="n">
         <v>0</v>
@@ -27867,11 +28379,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW130" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX130" s="20" t="n">
-        <v>0</v>
+      <c r="AW130" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX130" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY130" s="20" t="n">
         <v>0</v>
@@ -28074,11 +28590,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW131" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX131" s="20" t="n">
-        <v>0</v>
+      <c r="AW131" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX131" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY131" s="20" t="n">
         <v>0</v>
@@ -28281,11 +28801,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW132" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX132" s="20" t="n">
-        <v>1</v>
+      <c r="AW132" s="20" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="AX132" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
       </c>
       <c r="AY132" s="20" t="n">
         <v>0</v>
@@ -28485,11 +29009,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW133" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX133" s="20" t="n">
-        <v>0</v>
+      <c r="AW133" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX133" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY133" s="20" t="n">
         <v>0</v>
@@ -28687,11 +29215,15 @@
           <t>FN</t>
         </is>
       </c>
-      <c r="AW134" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX134" s="20" t="n">
-        <v>1</v>
+      <c r="AW134" s="20" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="AX134" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
       </c>
       <c r="AY134" s="20" t="n">
         <v>0</v>
@@ -28899,11 +29431,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW135" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX135" s="20" t="n">
-        <v>0</v>
+      <c r="AW135" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX135" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY135" s="20" t="n">
         <v>0</v>
@@ -29111,11 +29647,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW136" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX136" s="20" t="n">
-        <v>0</v>
+      <c r="AW136" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX136" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY136" s="20" t="n">
         <v>1</v>
@@ -29323,11 +29863,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW137" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX137" s="20" t="n">
-        <v>1</v>
+      <c r="AW137" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="AX137" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
       </c>
       <c r="AY137" s="20" t="n">
         <v>0</v>
@@ -29535,11 +30079,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW138" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX138" s="20" t="n">
-        <v>0</v>
+      <c r="AW138" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX138" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY138" s="20" t="n">
         <v>0</v>
@@ -29737,11 +30285,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW139" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX139" s="20" t="n">
-        <v>0</v>
+      <c r="AW139" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX139" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY139" s="20" t="n">
         <v>0</v>
@@ -29944,11 +30496,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW140" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX140" s="20" t="n">
-        <v>0</v>
+      <c r="AW140" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX140" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY140" s="20" t="n">
         <v>0</v>
@@ -30156,11 +30712,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW141" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX141" s="20" t="n">
-        <v>0</v>
+      <c r="AW141" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX141" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY141" s="20" t="n">
         <v>0</v>
@@ -30367,11 +30927,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW142" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX142" s="20" t="n">
-        <v>0</v>
+      <c r="AW142" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX142" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY142" s="20" t="n">
         <v>0</v>
@@ -30573,11 +31137,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW143" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX143" s="20" t="n">
-        <v>0</v>
+      <c r="AW143" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="AX143" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY143" s="20" t="n">
         <v>1</v>
@@ -30774,11 +31342,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW144" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX144" s="20" t="n">
-        <v>0</v>
+      <c r="AW144" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX144" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY144" s="20" t="n">
         <v>0</v>
@@ -30975,11 +31547,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW145" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX145" s="20" t="n">
-        <v>0</v>
+      <c r="AW145" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX145" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY145" s="20" t="n">
         <v>0</v>
@@ -31176,11 +31752,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW146" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX146" s="20" t="n">
-        <v>0</v>
+      <c r="AW146" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX146" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY146" s="20" t="n">
         <v>0</v>
@@ -31378,11 +31958,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW147" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX147" s="20" t="n">
-        <v>0</v>
+      <c r="AW147" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX147" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY147" s="20" t="n">
         <v>0</v>
@@ -31584,11 +32168,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW148" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX148" s="20" t="n">
-        <v>0</v>
+      <c r="AW148" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX148" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY148" s="20" t="n">
         <v>0</v>
@@ -31785,11 +32373,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW149" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX149" s="20" t="n">
-        <v>0</v>
+      <c r="AW149" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="AX149" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY149" s="20" t="n">
         <v>1</v>
@@ -31989,11 +32581,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW150" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX150" s="20" t="n">
-        <v>0</v>
+      <c r="AW150" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX150" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY150" s="20" t="n">
         <v>0</v>
@@ -32190,11 +32786,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW151" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX151" s="20" t="n">
-        <v>0</v>
+      <c r="AW151" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX151" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY151" s="20" t="n">
         <v>0</v>
@@ -32396,11 +32996,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW152" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX152" s="20" t="n">
-        <v>0</v>
+      <c r="AW152" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="AX152" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY152" s="20" t="n">
         <v>0</v>
@@ -32602,11 +33206,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW153" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX153" s="20" t="n">
-        <v>0</v>
+      <c r="AW153" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX153" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY153" s="20" t="n">
         <v>0</v>
@@ -32809,11 +33417,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW154" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX154" s="20" t="n">
-        <v>0</v>
+      <c r="AW154" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX154" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY154" s="20" t="n">
         <v>0</v>
@@ -33016,11 +33628,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX155" s="20" t="n">
-        <v>0</v>
+      <c r="AW155" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX155" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY155" s="20" t="n">
         <v>0</v>
@@ -33223,11 +33839,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW156" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX156" s="20" t="n">
-        <v>0</v>
+      <c r="AW156" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX156" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY156" s="20" t="n">
         <v>0</v>
@@ -33430,11 +34050,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW157" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX157" s="20" t="n">
-        <v>0</v>
+      <c r="AW157" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX157" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY157" s="20" t="n">
         <v>1</v>
@@ -33637,11 +34261,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW158" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX158" s="20" t="n">
-        <v>0</v>
+      <c r="AW158" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX158" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY158" s="20" t="n">
         <v>1</v>
@@ -33844,11 +34472,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW159" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX159" s="20" t="n">
-        <v>0</v>
+      <c r="AW159" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX159" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY159" s="20" t="n">
         <v>0</v>
@@ -34051,11 +34683,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW160" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX160" s="20" t="n">
-        <v>0</v>
+      <c r="AW160" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX160" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY160" s="20" t="n">
         <v>1</v>
@@ -34253,11 +34889,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW161" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX161" s="20" t="n">
-        <v>0</v>
+      <c r="AW161" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX161" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY161" s="20" t="n">
         <v>0</v>
@@ -34455,11 +35095,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW162" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX162" s="20" t="n">
-        <v>0</v>
+      <c r="AW162" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX162" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY162" s="20" t="n">
         <v>0</v>
@@ -34662,11 +35306,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW163" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX163" s="20" t="n">
-        <v>0</v>
+      <c r="AW163" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="AX163" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY163" s="20" t="n">
         <v>1</v>
@@ -34869,11 +35517,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW164" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX164" s="20" t="n">
-        <v>0</v>
+      <c r="AW164" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX164" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY164" s="20" t="n">
         <v>0</v>
@@ -35071,11 +35723,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW165" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX165" s="20" t="n">
-        <v>1</v>
+      <c r="AW165" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="AX165" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
       </c>
       <c r="AY165" s="20" t="n">
         <v>0</v>
@@ -35278,11 +35934,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW166" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX166" s="20" t="n">
-        <v>0</v>
+      <c r="AW166" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX166" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY166" s="20" t="n">
         <v>0</v>
@@ -35485,11 +36145,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW167" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX167" s="20" t="n">
-        <v>0</v>
+      <c r="AW167" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX167" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY167" s="20" t="n">
         <v>0</v>
@@ -35692,11 +36356,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW168" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX168" s="20" t="n">
-        <v>0</v>
+      <c r="AW168" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="AX168" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY168" s="20" t="n">
         <v>0</v>
@@ -35898,11 +36566,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW169" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX169" s="20" t="n">
-        <v>0</v>
+      <c r="AW169" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX169" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY169" s="20" t="n">
         <v>0</v>
@@ -36105,11 +36777,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW170" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX170" s="20" t="n">
-        <v>0</v>
+      <c r="AW170" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX170" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY170" s="20" t="n">
         <v>1</v>
@@ -36312,11 +36988,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW171" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX171" s="20" t="n">
-        <v>0</v>
+      <c r="AW171" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX171" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY171" s="20" t="n">
         <v>0</v>
@@ -36514,11 +37194,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW172" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX172" s="20" t="n">
-        <v>0</v>
+      <c r="AW172" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX172" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY172" s="20" t="n">
         <v>0</v>
@@ -36721,11 +37405,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW173" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX173" s="20" t="n">
-        <v>0</v>
+      <c r="AW173" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX173" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY173" s="20" t="n">
         <v>0</v>
@@ -36923,11 +37611,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW174" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX174" s="20" t="n">
-        <v>0</v>
+      <c r="AW174" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX174" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY174" s="20" t="n">
         <v>0</v>
@@ -37125,11 +37817,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW175" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX175" s="20" t="n">
-        <v>0</v>
+      <c r="AW175" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX175" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY175" s="20" t="n">
         <v>0</v>
@@ -37325,11 +38021,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW176" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX176" s="20" t="n">
-        <v>0</v>
+      <c r="AW176" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX176" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
       </c>
       <c r="AY176" s="20" t="n">
         <v>0</v>
@@ -37528,11 +38228,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW177" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX177" s="20" t="n">
-        <v>0</v>
+      <c r="AW177" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="AX177" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY177" s="20" t="n">
         <v>0</v>
@@ -37741,11 +38445,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW178" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX178" s="20" t="n">
-        <v>0</v>
+      <c r="AW178" s="20" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="AX178" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY178" s="20" t="n">
         <v>1</v>
@@ -37959,11 +38667,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW179" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX179" s="20" t="n">
-        <v>0</v>
+      <c r="AW179" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX179" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY179" s="20" t="n">
         <v>0</v>
@@ -38167,11 +38879,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW180" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX180" s="20" t="n">
-        <v>0</v>
+      <c r="AW180" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX180" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY180" s="20" t="n">
         <v>0</v>
@@ -38375,11 +39091,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW181" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX181" s="20" t="n">
-        <v>0</v>
+      <c r="AW181" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX181" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY181" s="20" t="n">
         <v>0</v>
@@ -38583,11 +39303,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW182" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX182" s="20" t="n">
-        <v>0</v>
+      <c r="AW182" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX182" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY182" s="20" t="n">
         <v>0</v>
@@ -38791,11 +39515,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW183" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX183" s="20" t="n">
-        <v>0</v>
+      <c r="AW183" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX183" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY183" s="20" t="n">
         <v>0</v>
@@ -39004,11 +39732,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW184" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX184" s="20" t="n">
-        <v>0</v>
+      <c r="AW184" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX184" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY184" s="20" t="n">
         <v>0</v>
@@ -39212,11 +39944,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW185" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX185" s="20" t="n">
-        <v>0</v>
+      <c r="AW185" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX185" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY185" s="20" t="n">
         <v>0</v>
@@ -39420,11 +40156,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW186" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX186" s="20" t="n">
-        <v>0</v>
+      <c r="AW186" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX186" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY186" s="20" t="n">
         <v>0</v>
@@ -39633,11 +40373,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW187" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX187" s="20" t="n">
-        <v>0</v>
+      <c r="AW187" s="20" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="AX187" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY187" s="20" t="n">
         <v>1</v>
@@ -39851,11 +40595,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW188" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX188" s="20" t="n">
-        <v>0</v>
+      <c r="AW188" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX188" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY188" s="20" t="n">
         <v>0</v>
@@ -40064,11 +40812,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW189" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX189" s="20" t="n">
-        <v>0</v>
+      <c r="AW189" s="20" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="AX189" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY189" s="20" t="n">
         <v>0</v>
@@ -40272,11 +41024,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW190" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX190" s="20" t="n">
-        <v>0</v>
+      <c r="AW190" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX190" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY190" s="20" t="n">
         <v>0</v>
@@ -40480,11 +41236,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW191" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX191" s="20" t="n">
-        <v>0</v>
+      <c r="AW191" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX191" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY191" s="20" t="n">
         <v>0</v>
@@ -40693,11 +41453,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW192" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX192" s="20" t="n">
-        <v>0</v>
+      <c r="AW192" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="AX192" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY192" s="20" t="n">
         <v>0</v>
@@ -40911,11 +41675,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW193" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX193" s="20" t="n">
-        <v>0</v>
+      <c r="AW193" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX193" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY193" s="20" t="n">
         <v>0</v>
@@ -41119,11 +41887,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW194" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX194" s="20" t="n">
-        <v>0</v>
+      <c r="AW194" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX194" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY194" s="20" t="n">
         <v>0</v>
@@ -41327,11 +42099,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW195" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX195" s="20" t="n">
-        <v>0</v>
+      <c r="AW195" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX195" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY195" s="20" t="n">
         <v>0</v>
@@ -41540,11 +42316,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW196" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX196" s="20" t="n">
-        <v>0</v>
+      <c r="AW196" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX196" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY196" s="20" t="n">
         <v>0</v>
@@ -41753,11 +42533,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW197" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX197" s="20" t="n">
-        <v>0</v>
+      <c r="AW197" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX197" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY197" s="20" t="n">
         <v>0</v>
@@ -41966,11 +42750,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW198" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX198" s="20" t="n">
-        <v>0</v>
+      <c r="AW198" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="AX198" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY198" s="20" t="n">
         <v>1</v>
@@ -42184,11 +42972,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW199" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX199" s="20" t="n">
-        <v>1</v>
+      <c r="AW199" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="AX199" s="20" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
       </c>
       <c r="AY199" s="20" t="n">
         <v>1</v>
@@ -42402,11 +43194,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW200" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX200" s="20" t="n">
-        <v>0</v>
+      <c r="AW200" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX200" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY200" s="20" t="n">
         <v>0</v>
@@ -42615,11 +43411,15 @@
           <t>TN</t>
         </is>
       </c>
-      <c r="AW201" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX201" s="20" t="n">
-        <v>0</v>
+      <c r="AW201" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="AX201" s="20" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
       </c>
       <c r="AY201" s="20" t="n">
         <v>0</v>

</xml_diff>